<commit_message>
TMT0072233_VerifyActivityIsLinkedToTheRelatedEngagement - Initial - 24 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51843D-3136-492E-8B7B-58A6972F3C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35038B31-C9A2-46D1-B7DF-46F0F537CA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
+    <sheet name="AddOpportunity" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>Users</t>
   </si>
@@ -110,6 +111,153 @@
   </si>
   <si>
     <t>OpportunityCFTest</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>JobType</t>
+  </si>
+  <si>
+    <t>IndustryGroup/HLSector</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>AdditionalClient</t>
+  </si>
+  <si>
+    <t>AdditonalSubject</t>
+  </si>
+  <si>
+    <t>ReferralType</t>
+  </si>
+  <si>
+    <t>NonPublicInfo</t>
+  </si>
+  <si>
+    <t>BeneficialOwner</t>
+  </si>
+  <si>
+    <t>PrimaryOffice</t>
+  </si>
+  <si>
+    <t>LegalEntity</t>
+  </si>
+  <si>
+    <t>DisclosureStatus</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Retainer</t>
+  </si>
+  <si>
+    <t>MonthlyFee</t>
+  </si>
+  <si>
+    <t>ContingentFee</t>
+  </si>
+  <si>
+    <t>ClientOwnership</t>
+  </si>
+  <si>
+    <t>SubjectOwnership</t>
+  </si>
+  <si>
+    <t>SICCode</t>
+  </si>
+  <si>
+    <t>OpportunityDescription</t>
+  </si>
+  <si>
+    <t>ReferralContact</t>
+  </si>
+  <si>
+    <t>Agreement</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>RecordType</t>
+  </si>
+  <si>
+    <t>FASJobType</t>
+  </si>
+  <si>
+    <t>MarketCap</t>
+  </si>
+  <si>
+    <t>Fee</t>
+  </si>
+  <si>
+    <t>StdUser</t>
+  </si>
+  <si>
+    <t>WomenLed</t>
+  </si>
+  <si>
+    <t>Techno Coatings, Inc.</t>
+  </si>
+  <si>
+    <t>Buyside</t>
+  </si>
+  <si>
+    <t>CSDN-0000002536</t>
+  </si>
+  <si>
+    <t>Dealership &amp; Rental Services</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>HL Capital, Inc.</t>
+  </si>
+  <si>
+    <t>Do Not Disclose</t>
+  </si>
+  <si>
+    <t>Emre Abale</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Public Equity</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Chris Lord</t>
+  </si>
+  <si>
+    <t>Yes, separate signed agreement</t>
+  </si>
+  <si>
+    <t>Cleared</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -159,11 +307,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -591,4 +743,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
+  <dimension ref="A1:AD2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mid - TMT0072233_VerifyActivityIsLinkedToTheRelatedEngagement - 24 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35038B31-C9A2-46D1-B7DF-46F0F537CA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB2747-078F-4CCB-9D96-3DA00A8B34FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
-  <si>
-    <t>Users</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Type</t>
   </si>
@@ -80,9 +77,6 @@
     <t>Meeting Notes 1</t>
   </si>
   <si>
-    <t>Thomas Bailey</t>
-  </si>
-  <si>
     <t>ContactName</t>
   </si>
   <si>
@@ -258,6 +252,18 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>CaoUser</t>
+  </si>
+  <si>
+    <t>Gemma Hardy</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>Sahil Mittal</t>
   </si>
 </sst>
 </file>
@@ -597,25 +603,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -640,24 +653,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -688,54 +701,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -760,186 +773,186 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>59</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>60</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>64</v>
       </c>
-      <c r="S2" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" t="s">
         <v>65</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
         <v>70</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Opportunities - Mid - 24 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB2747-078F-4CCB-9D96-3DA00A8B34FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA5B398-40D5-4427-82B9-7E520E5AD624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Final - TMT0072233_VerifyActivityIsLinkedToTheRelatedEngagement - 24 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA5B398-40D5-4427-82B9-7E520E5AD624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A5CFD1-FF87-4DB6-BE1A-62B550C6F893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="10" r:id="rId2"/>
     <sheet name="Activity" sheetId="11" r:id="rId3"/>
     <sheet name="AddOpportunity" sheetId="12" r:id="rId4"/>
+    <sheet name="AddContact" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -264,6 +265,45 @@
   </si>
   <si>
     <t>Sahil Mittal</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Type1</t>
+  </si>
+  <si>
+    <t>ClientType</t>
+  </si>
+  <si>
+    <t>Contact2</t>
+  </si>
+  <si>
+    <t>Type2</t>
+  </si>
+  <si>
+    <t>HLContact</t>
+  </si>
+  <si>
+    <t>Board of Directors</t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Emma Watson</t>
+  </si>
+  <si>
+    <t>Sonika Goyal</t>
   </si>
 </sst>
 </file>
@@ -762,7 +802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -958,4 +998,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial - 25 Sep 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A5CFD1-FF87-4DB6-BE1A-62B550C6F893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B35B12-E771-4778-9CBB-900E41137CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -90,12 +90,6 @@
     <t>Activity Test External Contact</t>
   </si>
   <si>
-    <t>Company Discussed Meeting</t>
-  </si>
-  <si>
-    <t>Company Discussed Meeting Description</t>
-  </si>
-  <si>
     <t>CompanyDiscussed</t>
   </si>
   <si>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t>Sonika Goyal</t>
+  </si>
+  <si>
+    <t>Engagement Discussed Meeting</t>
+  </si>
+  <si>
+    <t>Engagement Discussed Meeting Description</t>
   </si>
 </sst>
 </file>
@@ -657,18 +657,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,10 +759,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -779,16 +779,16 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -813,186 +813,186 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>57</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>58</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>62</v>
       </c>
-      <c r="S2" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" t="s">
         <v>63</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>64</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>65</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>66</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>67</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" t="s">
         <v>68</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33474F8B-FFCF-4033-9E95-D6C9D3A8099C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -1012,54 +1012,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
27 Jan 2025 - Mid
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B35B12-E771-4778-9CBB-900E41137CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753B053-8406-42ED-AEB1-6A8F7F95FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3516" yWindow="1500" windowWidth="19416" windowHeight="10740" tabRatio="468" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Type</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Buyside</t>
-  </si>
-  <si>
-    <t>CSDN-0000002536</t>
   </si>
   <si>
     <t>Dealership &amp; Rental Services</t>
@@ -657,18 +654,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -723,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB9990D-2177-413E-8716-FEF5A04433C7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -779,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -802,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,85 +911,85 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
         <v>53</v>
       </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>56</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>57</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="S2" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="S2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" t="s">
         <v>61</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>62</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>63</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>64</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>66</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" t="s">
         <v>67</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1012,54 +1009,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Data change- 12 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
+++ b/TestData/TMTC0032668_VerifyActivityIsLinkedToTheRelatedEngagement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753B053-8406-42ED-AEB1-6A8F7F95FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E147C6-F977-4E35-8887-4C675BB2F35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3516" yWindow="1500" windowWidth="19416" windowHeight="10740" tabRatio="468" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="468" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t>CaoUser</t>
   </si>
   <si>
-    <t>Gemma Hardy</t>
-  </si>
-  <si>
     <t>Admin User</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Engagement Discussed Meeting Description</t>
+  </si>
+  <si>
+    <t>Giselle Segura</t>
   </si>
 </sst>
 </file>
@@ -642,30 +642,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -682,13 +682,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -699,7 +699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -724,19 +724,19 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -762,12 +762,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -776,7 +776,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -799,16 +799,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -900,7 +900,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1005,58 +1005,58 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>79</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
       <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>82</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>